<commit_message>
Updated the google docs
</commit_message>
<xml_diff>
--- a/Project_Files/TestMatrix/Test Matrix.xlsx
+++ b/Project_Files/TestMatrix/Test Matrix.xlsx
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="68">
   <si>
     <t>Requirement #</t>
   </si>
@@ -416,12 +416,27 @@
   <si>
     <t>Graffiti Reporting (GR) Requirements (Status Report)</t>
   </si>
+  <si>
+    <t>REQUIREMENTS MAPPING:</t>
+  </si>
+  <si>
+    <t>Data Requirements → Information Class</t>
+  </si>
+  <si>
+    <t>User Access Requirements → UserAccess class</t>
+  </si>
+  <si>
+    <t>UI Requirments → Tkinter/html</t>
+  </si>
+  <si>
+    <t>Performance Requirements → Testing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -432,6 +447,10 @@
     </font>
     <font>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -454,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -466,6 +485,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -2243,7 +2268,9 @@
     </row>
     <row r="41">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="B41" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2271,7 +2298,9 @@
     </row>
     <row r="42">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
+      <c r="B42" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2299,7 +2328,9 @@
     </row>
     <row r="43">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="B43" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2327,7 +2358,9 @@
     </row>
     <row r="44">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="B44" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2355,7 +2388,9 @@
     </row>
     <row r="45">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="B45" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>

</xml_diff>